<commit_message>
Added Sequence generator for TS401
</commit_message>
<xml_diff>
--- a/test/UnitTest 00.xlsx
+++ b/test/UnitTest 00.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="Workbook________" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
   </bookViews>
   <sheets>
     <sheet name="Test_1.2" sheetId="4" r:id="rId1"/>
+    <sheet name="TS_1.2" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="53">
   <si>
     <t>Target</t>
   </si>
@@ -37,9 +38,6 @@
     <t>CAN_B_KrRSh1_BEU_ Vehx</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>CAN_B_KrRSh2_BEU_ Vehx</t>
   </si>
   <si>
@@ -97,9 +95,6 @@
     <t>STEP 14</t>
   </si>
   <si>
-    <t>B_Wrong_pos_cocks_train_normal_mode</t>
-  </si>
-  <si>
     <t>Right conditions</t>
   </si>
   <si>
@@ -137,13 +132,55 @@
   </si>
   <si>
     <t>DELAY</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>B_VarToCheck1</t>
+  </si>
+  <si>
+    <t>B_VarToCheck0</t>
+  </si>
+  <si>
+    <t>B_VarToCheck2</t>
+  </si>
+  <si>
+    <t>Location1</t>
+  </si>
+  <si>
+    <t>Location2</t>
+  </si>
+  <si>
+    <t>Location3</t>
+  </si>
+  <si>
+    <t>Location4</t>
+  </si>
+  <si>
+    <t>Location5</t>
+  </si>
+  <si>
+    <t>Location6</t>
+  </si>
+  <si>
+    <t>Location7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +204,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +239,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -200,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -218,9 +282,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -341,7 +408,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B15:Q15" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B15:Q17" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="16">
     <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
@@ -388,9 +455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +495,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -500,7 +567,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -677,76 +744,76 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
         <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -766,43 +833,43 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>20</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>21</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>22</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>23</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>24</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>25</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -811,7 +878,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -826,10 +893,10 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -843,10 +910,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -860,10 +927,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -877,10 +944,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -894,10 +961,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -908,10 +975,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -925,40 +992,34 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" t="s">
         <v>37</v>
       </c>
-      <c r="I13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
+      <c r="B15" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
       <c r="H15">
         <v>0</v>
       </c>
@@ -987,6 +1048,40 @@
         <v>0</v>
       </c>
       <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="O17">
         <v>1</v>
       </c>
     </row>
@@ -1001,4 +1096,850 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Worksheet____2"/>
+  <dimension ref="D1:Q42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+    </row>
+    <row r="2" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+    </row>
+    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+    </row>
+    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" t="s">
+        <v>43</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" t="s">
+        <v>45</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" t="s">
+        <v>44</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" t="s">
+        <v>44</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+    </row>
+    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" t="s">
+        <v>44</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+    </row>
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" t="s">
+        <v>44</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>40</v>
+      </c>
+      <c r="L37" t="s">
+        <v>45</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+    </row>
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" t="s">
+        <v>44</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D40" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L41" t="s">
+        <v>44</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="K38:Q38"/>
+    <mergeCell ref="F40:J40"/>
+    <mergeCell ref="K40:Q40"/>
+    <mergeCell ref="F42:J42"/>
+    <mergeCell ref="K42:Q42"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="K29:Q29"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="K31:Q31"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="K34:Q34"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="K21:Q21"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="K25:Q25"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="K27:Q27"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="K14:Q14"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="K16:Q16"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="K18:Q18"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="K9:Q9"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="K12:Q12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated referential to test result of compairison.
</commit_message>
<xml_diff>
--- a/test/UnitTest 00.xlsx
+++ b/test/UnitTest 00.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="45">
   <si>
     <t>Target</t>
   </si>
@@ -98,39 +98,9 @@
     <t>Right conditions</t>
   </si>
   <si>
-    <t>КрРШ1(БТО) in a faulty state (closed)</t>
-  </si>
-  <si>
-    <t>КрРШ2(БТО) in a faulty state (closed)</t>
-  </si>
-  <si>
-    <t>КрРШ3(БТО) in a faulty state (closed)</t>
-  </si>
-  <si>
-    <t>КрРШ4(БТО) in a faulty state (opened)</t>
-  </si>
-  <si>
-    <t>КрРШ9(БТО) in a faulty state (closed)</t>
-  </si>
-  <si>
-    <t>КрРШ2(MТО) in a faulty state (closed)</t>
-  </si>
-  <si>
-    <t>Speed is higher than 3kph</t>
-  </si>
-  <si>
     <t>Test 1.2</t>
   </si>
   <si>
-    <t>4000</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>7000</t>
-  </si>
-  <si>
     <t>DELAY</t>
   </si>
   <si>
@@ -155,34 +125,31 @@
     <t>B_VarToCheck2</t>
   </si>
   <si>
-    <t>Location1</t>
-  </si>
-  <si>
-    <t>Location2</t>
-  </si>
-  <si>
-    <t>Location3</t>
-  </si>
-  <si>
-    <t>Location4</t>
-  </si>
-  <si>
-    <t>Location5</t>
-  </si>
-  <si>
-    <t>Location6</t>
-  </si>
-  <si>
-    <t>Location7</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>I:CAN_B_KrRSh9_BEU_ Vehx</t>
-  </si>
-  <si>
-    <t>DT:CAN_B_KrRSh3_BEU_ Vehx</t>
+    <t>Application_TrTrans/Embedded/Control_Command/FBS/TFE/tfe_aht_trtrans1/tfe_aht_f15_trtrans1</t>
+  </si>
+  <si>
+    <t>B_CabAct</t>
+  </si>
+  <si>
+    <t>BY_NumSec</t>
+  </si>
+  <si>
+    <t>P_TpTime</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>BY_SelVehHHT_UM</t>
+  </si>
+  <si>
+    <t>B_HHTOpenState_Veh1_DDU</t>
+  </si>
+  <si>
+    <t>Actions to perform</t>
+  </si>
+  <si>
+    <t>Checks to perform</t>
   </si>
 </sst>
 </file>
@@ -296,9 +263,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -313,9 +283,6 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -392,49 +359,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:Q13" totalsRowCount="1">
-  <autoFilter ref="B5:Q12"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:D9" totalsRowCount="1">
+  <autoFilter ref="B5:D8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="STEP 1"/>
-    <tableColumn id="4" name="STEP 2" totalsRowLabel="4000"/>
-    <tableColumn id="5" name="STEP 3"/>
-    <tableColumn id="6" name="STEP 4"/>
-    <tableColumn id="7" name="STEP 5"/>
-    <tableColumn id="8" name="STEP 6" totalsRowLabel="5000"/>
-    <tableColumn id="9" name="STEP 7"/>
-    <tableColumn id="10" name="STEP 8"/>
-    <tableColumn id="11" name="STEP 9"/>
-    <tableColumn id="12" name="STEP 10"/>
-    <tableColumn id="13" name="STEP 11" totalsRowLabel="7000"/>
-    <tableColumn id="14" name="STEP 12"/>
-    <tableColumn id="15" name="STEP 13"/>
-    <tableColumn id="16" name="STEP 14"/>
+    <tableColumn id="3" name="STEP 1" totalsRowLabel="2000"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B15:Q17" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="16">
-    <tableColumn id="1" name="Target" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B11:D12" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="0"/>
-    <tableColumn id="4" name="Colonne1"/>
-    <tableColumn id="5" name="Colonne2"/>
-    <tableColumn id="6" name="Colonne3"/>
-    <tableColumn id="7" name="Colonne4"/>
-    <tableColumn id="8" name="Colonne5"/>
-    <tableColumn id="9" name="Colonne6"/>
-    <tableColumn id="10" name="Colonne7"/>
-    <tableColumn id="11" name="Colonne8"/>
-    <tableColumn id="12" name="Colonne9"/>
-    <tableColumn id="13" name="Colonne10"/>
-    <tableColumn id="14" name="Colonne11"/>
-    <tableColumn id="15" name="Colonne12"/>
-    <tableColumn id="16" name="Colonne13"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -464,9 +405,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -504,7 +445,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -576,7 +517,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -753,31 +694,37 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -785,50 +732,11 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -841,278 +749,75 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="42" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1137,7 +842,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D1" s="6" t="s">
@@ -1159,7 +864,7 @@
     </row>
     <row r="2" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1174,10 +879,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1188,7 +893,7 @@
     </row>
     <row r="3" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -1202,7 +907,7 @@
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -1216,7 +921,7 @@
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -1230,7 +935,7 @@
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -1244,7 +949,7 @@
     </row>
     <row r="7" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -1258,7 +963,7 @@
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
@@ -1290,7 +995,7 @@
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -1305,10 +1010,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1319,7 +1024,7 @@
     </row>
     <row r="11" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="I11">
         <v>4000</v>
@@ -1345,7 +1050,7 @@
     </row>
     <row r="13" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -1360,10 +1065,10 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L13" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1392,7 +1097,7 @@
     </row>
     <row r="15" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s">
         <v>7</v>
@@ -1404,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L15" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1433,7 +1138,7 @@
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
         <v>7</v>
@@ -1445,10 +1150,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L17" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1477,7 +1182,7 @@
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -1489,10 +1194,10 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L19" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1503,7 +1208,7 @@
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="I20">
         <v>5000</v>
@@ -1529,7 +1234,7 @@
     </row>
     <row r="22" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -1541,10 +1246,10 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L22" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -1555,10 +1260,10 @@
     </row>
     <row r="23" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -1569,10 +1274,10 @@
     </row>
     <row r="24" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K24" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L24" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -1598,7 +1303,7 @@
     </row>
     <row r="26" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -1610,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -1642,7 +1347,7 @@
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -1654,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -1686,7 +1391,7 @@
     </row>
     <row r="30" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1698,10 +1403,10 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L30" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -1730,7 +1435,7 @@
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
@@ -1742,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L32" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -1756,7 +1461,7 @@
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="I33">
         <v>7000</v>
@@ -1782,7 +1487,7 @@
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G35" t="s">
         <v>11</v>
@@ -1794,10 +1499,10 @@
         <v>1</v>
       </c>
       <c r="K35" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L35" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -1808,10 +1513,10 @@
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L36" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -1822,10 +1527,10 @@
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K37" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L37" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -1851,7 +1556,7 @@
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G39" t="s">
         <v>12</v>
@@ -1863,10 +1568,10 @@
         <v>1</v>
       </c>
       <c r="K39" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L39" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M39">
         <v>0</v>
@@ -1895,7 +1600,7 @@
     </row>
     <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G41" t="s">
         <v>12</v>
@@ -1907,10 +1612,10 @@
         <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L41" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M41">
         <v>0</v>
@@ -1921,7 +1626,7 @@
     </row>
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42" s="6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="9"/>
@@ -1939,36 +1644,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="K38:Q38"/>
+    <mergeCell ref="F40:J40"/>
+    <mergeCell ref="K40:Q40"/>
+    <mergeCell ref="F42:J42"/>
+    <mergeCell ref="K42:Q42"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="K29:Q29"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="K31:Q31"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="K34:Q34"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="K21:Q21"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="K25:Q25"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="K27:Q27"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="K14:Q14"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="K16:Q16"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="K18:Q18"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:Q1"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="K9:Q9"/>
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="K12:Q12"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="K14:Q14"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="K16:Q16"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="K18:Q18"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="K21:Q21"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="K25:Q25"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="K27:Q27"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="K29:Q29"/>
-    <mergeCell ref="F31:J31"/>
-    <mergeCell ref="K31:Q31"/>
-    <mergeCell ref="F34:J34"/>
-    <mergeCell ref="K34:Q34"/>
-    <mergeCell ref="F38:J38"/>
-    <mergeCell ref="K38:Q38"/>
-    <mergeCell ref="F40:J40"/>
-    <mergeCell ref="K40:Q40"/>
-    <mergeCell ref="F42:J42"/>
-    <mergeCell ref="K42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>